<commit_message>
readd venturis to pressure drop
</commit_message>
<xml_diff>
--- a/Pressure drop/fluid_components.xlsx
+++ b/Pressure drop/fluid_components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\PSPL_Rocket_A\Pressure drop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3E4F2D-F35E-4D25-A09A-C7A1FBE8E81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC95E6AC-68E1-4F0F-96CD-074FCE1F4575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Straight Tube</t>
   </si>
   <si>
-    <t>Part 2</t>
-  </si>
-  <si>
     <t>Venturi</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Bend</t>
   </si>
   <si>
-    <t>Part 22</t>
-  </si>
-  <si>
     <t>Injector</t>
   </si>
   <si>
@@ -128,6 +122,12 @@
   </si>
   <si>
     <t>Part Type</t>
+  </si>
+  <si>
+    <t>LOx Venturi</t>
+  </si>
+  <si>
+    <t>Fuel Venturi</t>
   </si>
 </sst>
 </file>
@@ -604,10 +604,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,12 +623,12 @@
     <col min="10" max="10" width="30.7265625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -655,9 +655,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -679,31 +679,31 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L3" s="7" t="s">
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="9">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="9">
         <v>0.75</v>
       </c>
-      <c r="T3" s="9">
+      <c r="I3" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="U3" s="9">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J3" s="9">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
@@ -725,12 +725,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="14"/>
@@ -751,9 +751,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -775,12 +775,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -791,9 +791,9 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -805,9 +805,9 @@
       <c r="I8" s="17"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>8</v>
@@ -829,12 +829,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="12">
         <v>90</v>
@@ -855,9 +855,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>8</v>
@@ -879,12 +879,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="12">
         <v>90</v>
@@ -905,9 +905,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>8</v>
@@ -929,12 +929,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="12">
         <v>90</v>
@@ -955,9 +955,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>8</v>
@@ -979,12 +979,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="12">
         <v>90</v>
@@ -1005,9 +1005,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>8</v>
@@ -1029,31 +1029,31 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="11">
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="11">
         <v>0.75</v>
       </c>
-      <c r="T18" s="11">
+      <c r="I18" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="U18" s="11">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J18" s="11">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>8</v>
@@ -1075,12 +1075,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="15"/>
@@ -1101,9 +1101,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>8</v>
@@ -1125,12 +1125,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>

</xml_diff>

<commit_message>
fix name and remove venturi
</commit_message>
<xml_diff>
--- a/Pressure drop/fluid_components.xlsx
+++ b/Pressure drop/fluid_components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\PSPL_Rocket_A\Pressure drop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC95E6AC-68E1-4F0F-96CD-074FCE1F4575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB713677-E2C8-479E-92E8-C6349F1D90DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,10 +604,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A8" sqref="A8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,7 +623,7 @@
     <col min="10" max="10" width="30.7265625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -655,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -679,29 +679,29 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="9">
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="9">
         <v>0.75</v>
       </c>
-      <c r="I3" s="9">
+      <c r="T3" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="J3" s="9">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U3" s="9">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
@@ -725,7 +725,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -751,7 +751,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -775,7 +775,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -791,7 +791,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -829,7 +829,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
@@ -855,7 +855,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
@@ -879,7 +879,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
@@ -905,7 +905,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
@@ -929,7 +929,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
@@ -955,7 +955,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>24</v>
       </c>
@@ -979,7 +979,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>30</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -1029,29 +1029,29 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="M18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="11">
+      <c r="N18" s="11"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="11">
         <v>0.75</v>
       </c>
-      <c r="I18" s="11">
+      <c r="T18" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="J18" s="11">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U18" s="11">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>26</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>32</v>
       </c>

</xml_diff>